<commit_message>
Created folders for prefabs and scripts
Created folders for prefabs and scripts
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0330\Documents\GitHub\JumpyStreetSGD285\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC56A6E7-AF01-4882-8CB7-5990E79E1AAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925F301E-2FDE-44E3-85BE-1CE6502534A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Jumpy Street</t>
   </si>
@@ -60,9 +60,6 @@
     <t>The procedural creation of platforms for the character to navigate in a sequential fashion.</t>
   </si>
   <si>
-    <t>The creation of a Main menu with instructions and credits screen.</t>
-  </si>
-  <si>
     <t>The creation of a UI system that keeps track of the player score and high scores.</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>Experiment with camera angles</t>
+  </si>
+  <si>
+    <t>The creation of a Main menu with instructions and credits screen. Also start UI creation for level.</t>
+  </si>
+  <si>
+    <t>Adding capability for controller to spawn object in hazardous zones and safe zones.</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,40 +300,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -469,6 +450,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -476,15 +463,38 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -501,16 +511,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FE176E1-7ACF-44EF-A514-EB363791678C}" name="Table1" displayName="Table1" ref="A3:D23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
-  <autoFilter ref="A3:D23" xr:uid="{59ED1BE4-E778-4B61-BB75-032C807B58B4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D23">
-    <sortCondition ref="B3:B23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FE176E1-7ACF-44EF-A514-EB363791678C}" name="Table1" displayName="Table1" ref="A3:D24" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:D24" xr:uid="{59ED1BE4-E778-4B61-BB75-032C807B58B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D24">
+    <sortCondition ref="B3:B24"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75E062D6-DFD7-41D5-A9BE-ABC5975A749B}" name="Features and Description" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{79FC60EC-1C78-4D9E-989B-E02064F1E89B}" name="Estimated Implementation" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E8F84168-71D0-49A6-A040-D9DC6F5EDFCF}" name="Assigned To" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C665A4A4-0634-4DD9-A0E6-3EB5C4422863}" name="Status" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{75E062D6-DFD7-41D5-A9BE-ABC5975A749B}" name="Features and Description" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{79FC60EC-1C78-4D9E-989B-E02064F1E89B}" name="Estimated Implementation" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E8F84168-71D0-49A6-A040-D9DC6F5EDFCF}" name="Assigned To" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C665A4A4-0634-4DD9-A0E6-3EB5C4422863}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -779,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -844,24 +854,24 @@
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="7" t="s">
@@ -870,10 +880,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="7" t="s">
@@ -882,10 +892,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="7" t="s">
@@ -894,10 +904,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="7" t="s">
@@ -906,46 +916,46 @@
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="7" t="s">
+    <row r="13" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7" t="s">
@@ -954,10 +964,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="7" t="s">
@@ -966,10 +976,10 @@
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="7" t="s">
@@ -978,10 +988,10 @@
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="7" t="s">
@@ -990,10 +1000,10 @@
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="7" t="s">
@@ -1002,7 +1012,7 @@
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>26</v>
@@ -1014,10 +1024,10 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="7" t="s">
@@ -1026,10 +1036,10 @@
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="7" t="s">
@@ -1037,29 +1047,41 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B9 B11:B20 B22:B23" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C7:C20 C22:C23" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B9 B23:B24 B11:B12 B14:B21" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C23:C24 C7:C12 C14:C21" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Use the dropdown menu to choose: Not implemented, In Progress or Done." sqref="D3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D24 D7:D12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated with assignments for tasks
Assigned different tasks
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0330\Documents\GitHub\JumpyStreetSGD285\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SPG_WorkSpace\JumpyStreetSGD285\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925F301E-2FDE-44E3-85BE-1CE6502534A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECFD51F-5491-4981-B412-DD8D7B9E3355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="2400" windowWidth="20385" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>Jumpy Street</t>
   </si>
@@ -57,18 +57,9 @@
     <t>Insert a row above to add more features to the list.</t>
   </si>
   <si>
-    <t>The procedural creation of platforms for the character to navigate in a sequential fashion.</t>
-  </si>
-  <si>
     <t>The creation of a UI system that keeps track of the player score and high scores.</t>
   </si>
   <si>
-    <t>Death zones that are on the front of obstacles to be avoided or in zones to be crossed.</t>
-  </si>
-  <si>
-    <t>Implemetation of obstacles and dead zones</t>
-  </si>
-  <si>
     <t>Implementation of impassable zones on either side of the terrain.</t>
   </si>
   <si>
@@ -145,6 +136,21 @@
   </si>
   <si>
     <t>Adding capability for controller to spawn object in hazardous zones and safe zones.</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Brennan</t>
+  </si>
+  <si>
+    <t>Death zones that are attached to objects</t>
+  </si>
+  <si>
+    <t>Implemetation of obstacles and dead zones to cross</t>
+  </si>
+  <si>
+    <t>Both?</t>
   </si>
 </sst>
 </file>
@@ -511,10 +517,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FE176E1-7ACF-44EF-A514-EB363791678C}" name="Table1" displayName="Table1" ref="A3:D24" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:D24" xr:uid="{59ED1BE4-E778-4B61-BB75-032C807B58B4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D24">
-    <sortCondition ref="B3:B24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FE176E1-7ACF-44EF-A514-EB363791678C}" name="Table1" displayName="Table1" ref="A3:D23" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:D23" xr:uid="{59ED1BE4-E778-4B61-BB75-032C807B58B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D23">
+    <sortCondition ref="B3:B23"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{75E062D6-DFD7-41D5-A9BE-ABC5975A749B}" name="Features and Description" dataDxfId="3"/>
@@ -789,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -854,13 +860,13 @@
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
@@ -868,220 +874,240 @@
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4"/>
       <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D17" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="D18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D20" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D22" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B9 B23:B24 B11:B12 B14:B21" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C23:C24 C7:C12 C14:C21" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B9 B22:B23 B11:B12 B14:B20" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C22:C23 C7:C12 C14:C20" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Use the dropdown menu to choose: Not implemented, In Progress or Done." sqref="D3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D24 D7:D12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D12 D14:D23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Names to project plan
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SPG_WorkSpace\JumpyStreetSGD285\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECFD51F-5491-4981-B412-DD8D7B9E3355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCEE74C-BB43-4193-8484-9378FA5DB3A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2325" yWindow="2400" windowWidth="20385" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Jumpy Street</t>
   </si>
   <si>
-    <t>Project Lead:</t>
-  </si>
-  <si>
     <t>Estimated Implementation</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Both?</t>
+  </si>
+  <si>
+    <t>Project Lead: Brennan Sullivan and Jacob Coleman</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -817,21 +817,21 @@
     </row>
     <row r="2" spans="1:4" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -839,7 +839,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -855,250 +855,250 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pause Screen to MainGame
added a pause screen and score panel to the MainGame scene.
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SPG_WorkSpace\JumpyStreetSGD285\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C6D14-76FE-4494-91F3-8753CED9A177}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475ED652-20D5-4F42-B3C4-AA299ABC5379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2325" yWindow="2400" windowWidth="20385" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>The ability for the player to jump between platforms or safe zones.</t>
   </si>
   <si>
-    <t>The ability for the charcter to move in cardinal directions and Jump (Camera is vertically fixed on player</t>
-  </si>
-  <si>
     <t>Blockers on safe zones</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Project Lead: Brennan Sullivan and Jacob Coleman</t>
+  </si>
+  <si>
+    <t>The ability for the charcter to move/jump in cardinal directions (Camera is vertically fixed on player</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -817,7 +817,7 @@
     </row>
     <row r="2" spans="1:4" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -860,13 +860,13 @@
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -874,13 +874,13 @@
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>4</v>
@@ -888,13 +888,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>5</v>
@@ -902,13 +902,13 @@
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
@@ -916,13 +916,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>4</v>
@@ -947,10 +947,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>4</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>4</v>
@@ -975,10 +975,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>4</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>4</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>4</v>
@@ -1017,10 +1017,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>4</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>4</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>4</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>4</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>4</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>4</v>

</xml_diff>